<commit_message>
`docs`: update example file
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\free-mind\games\admin\assets\l10n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\dart\arbexcel\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F20AB6-7B54-4111-8AC5-4B22B75E5F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E016D0-583B-40D0-9AE6-B078F3D4E212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="1776" windowWidth="15108" windowHeight="12888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>description</t>
   </si>
@@ -38,9 +32,6 @@
     <t>vi</t>
   </si>
   <si>
-    <t>common</t>
-  </si>
-  <si>
     <t>welcome</t>
   </si>
   <si>
@@ -59,9 +50,6 @@
     <t>Dashboard</t>
   </si>
   <si>
-    <t>campaign</t>
-  </si>
-  <si>
     <t>Campaigns</t>
   </si>
   <si>
@@ -219,6 +207,9 @@
   </si>
   <si>
     <t>Condition format: duplicate values</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -229,21 +220,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -251,7 +242,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +250,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -267,35 +258,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -303,7 +294,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -311,14 +302,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -326,14 +317,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +332,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,14 +340,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -770,7 +761,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -789,49 +780,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -846,11 +794,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0">
-  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="category"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="text"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D18" totalsRowShown="0">
+  <autoFilter ref="A1:D18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="description"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="en"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="vi"/>
@@ -1168,286 +1115,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+      <c r="C13" t="s">
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>38</v>
+      <c r="C14" t="s">
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:Z12 E16:Z1048576 F13:Z15">
+  <conditionalFormatting sqref="D1:Y12 D16:Y1048576 E13:Y15">
     <cfRule type="containsBlanks" dxfId="1" priority="5">
-      <formula>LEN(TRIM(E1))=0</formula>
+      <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,52 +1358,52 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.8984375" customWidth="1"/>
-    <col min="2" max="2" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>